<commit_message>
las graficas de las edades y una imagen
</commit_message>
<xml_diff>
--- a/antiguedad-matematica.xlsx
+++ b/antiguedad-matematica.xlsx
@@ -52,10 +52,10 @@
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Liberation Sans" fo:font-size="10pt" fo:language="es" fo:country="CU" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:language="es" fo:country="CU" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
   </office:automatic-styles>
@@ -67,7 +67,7 @@
         <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co5" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce1"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce5"/>
         <table:table-column table:style-name="co7" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2426,7 +2426,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="50081600809" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="50081600809" calcext:value-type="float">
             <text:p>50081600809</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2516,7 +2516,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Investigador Auxiliar</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="62101919699" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="62101919699" calcext:value-type="float">
             <text:p>62101919699</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2539,7 +2539,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="87081206903" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="87081206903" calcext:value-type="float">
             <text:p>87081206903</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2562,7 +2562,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Profesor Asistente</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="87042015226" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="87042015226" calcext:value-type="float">
             <text:p>87042015226</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2583,7 +2583,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="68081419509" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="68081419509" calcext:value-type="float">
             <text:p>68081419509</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2606,7 +2606,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>94102326118 </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2629,7 +2629,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Profesor Asistente</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="88070510186" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="88070510186" calcext:value-type="float">
             <text:p>88070510186</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2652,7 +2652,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="89110602981" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="89110602981" calcext:value-type="float">
             <text:p>89110602981</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2675,7 +2675,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="94090407004" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="94090407004" calcext:value-type="float">
             <text:p>94090407004</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2698,7 +2698,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Aspirante a Investigador</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="91092122263" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="91092122263" calcext:value-type="float">
             <text:p>91092122263</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2721,7 +2721,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="94042130823" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="94042130823" calcext:value-type="float">
             <text:p>94042130823</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2755,7 +2755,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="65091603195" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="65091603195" calcext:value-type="float">
             <text:p>65091603195</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2776,7 +2776,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="69070613995" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="69070613995" calcext:value-type="float">
             <text:p>69070613995</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2797,7 +2797,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="75032703172" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="75032703172" calcext:value-type="float">
             <text:p>75032703172</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2818,7 +2818,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>83081027581</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2839,7 +2839,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="90090928842" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="90090928842" calcext:value-type="float">
             <text:p>90090928842</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2862,7 +2862,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Instructor</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>91062846065 </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2883,7 +2883,7 @@
             <text:p>No Docente</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="float" office:value="92051727736" calcext:value-type="float">
+          <table:table-cell table:style-name="ce6" office:value-type="float" office:value="92051727736" calcext:value-type="float">
             <text:p>92051727736</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -2913,9 +2913,9 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
-    <dc:date>2024-08-05T09:11:52.427452712</dc:date>
-    <meta:editing-duration>PT43M54S</meta:editing-duration>
-    <meta:editing-cycles>9</meta:editing-cycles>
+    <dc:date>2024-08-22T19:49:57.295450714</dc:date>
+    <meta:editing-duration>PT1H22M13S</meta:editing-duration>
+    <meta:editing-cycles>10</meta:editing-cycles>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="811" meta:object-count="0"/>
   </office:meta>
@@ -2935,13 +2935,13 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">143</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">7</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">17</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">123</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -2950,7 +2950,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">852</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1301</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -3006,7 +3006,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAtQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">oAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -3049,19 +3049,21 @@
     <number:number-style style:name="N117P0" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N117P1" style:volatile="true">
       <number:text>-</number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N117P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
     </number:number-style>
     <number:text-style style:name="N117">
       <number:text> </number:text>
@@ -3071,86 +3073,84 @@
       <style:map style:condition="value()&lt;0" style:apply-style-name="N117P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N117P2"/>
     </number:text-style>
-    <number:number-style style:name="N113P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N113P1" style:volatile="true">
-      <number:text>-</number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N113P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:text-style style:name="N113">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N113P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N113P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N113P2"/>
-    </number:text-style>
-    <number:time-style style:name="N109">
+    <number:time-style style:name="N113">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:number-style style:name="N121P0" style:volatile="true">
+    <number:number-style style:name="N112P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N121">
+    <number:number-style style:name="N112">
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N112P0"/>
     </number:number-style>
-    <number:time-style style:name="N108" number:truncate-on-overflow="false">
+    <number:time-style style:name="N111" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:number-style style:name="N120P0" style:volatile="true">
+    <number:number-style style:name="N110P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N120">
+    <number:number-style style:name="N110">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N120P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N110P0"/>
     </number:number-style>
-    <number:time-style style:name="N107">
+    <number:time-style style:name="N109">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N119P0" style:volatile="true">
+    <number:number-style style:name="N121P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N121P1" style:volatile="true">
+      <number:text>-</number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N121P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:number-style>
+    <number:text-style style:name="N121">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N121P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N121P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N121P2"/>
+    </number:text-style>
+    <number:number-style style:name="N108P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N119">
+    <number:number-style style:name="N108">
       <number:text>-</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N119P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N108P0"/>
+    </number:number-style>
+    <number:number-style style:name="N107">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
+    <number:number-style style:name="N106P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
     <number:number-style style:name="N106">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
-    </number:number-style>
-    <number:number-style style:name="N118P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-    </number:number-style>
-    <number:number-style style:name="N118">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N118P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N106P0"/>
     </number:number-style>
     <number:number-style style:name="N105P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1"/>

</xml_diff>